<commit_message>
Added viz at bottom
</commit_message>
<xml_diff>
--- a/Honors_stats_updated_nov18_2.xlsx
+++ b/Honors_stats_updated_nov18_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EdwinReyesHerrera/Desktop/STAT112/stats112_finalproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F02D26-6080-424A-B719-528891196DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8963AA0A-FBB7-0649-BB77-DC5DF37CB514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2924,7 +2924,7 @@
         <v>2017</v>
       </c>
       <c r="N27" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="O27" t="s">
         <v>77</v>
@@ -4406,7 +4406,7 @@
         <v>22</v>
       </c>
       <c r="K51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L51">
         <v>2019</v>

</xml_diff>